<commit_message>
updated the heartrate into the gui
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2020-11-02" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2020-11-08" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2020-11-09" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2020-11-10" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1106,4 +1107,493 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01:38:44</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>84.61483623004834</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01:41:23</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>82.09468127949228</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09:21:53</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>89.30021772238722</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>09:35:17</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>94.56050200781256</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>09:36:59</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>92.57248194477947</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>09:43:12</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>94.81811911912854</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>09:47:16</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>96.61184229430469</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>09:53:50</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>94.65548776817448</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>09:54:29</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>95.39734931207116</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>09:59:30</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>95.39645256607388</v>
+      </c>
+      <c r="G11" t="n">
+        <v>66.23650871842609</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12:10:10</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>95.20561567862042</v>
+      </c>
+      <c r="G12" t="n">
+        <v>58.05271621944848</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12:14:45</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>96.11290914378348</v>
+      </c>
+      <c r="G13" t="n">
+        <v>74.2404288587264</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12:17:37</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>90.97632885109677</v>
+      </c>
+      <c r="G14" t="n">
+        <v>75.00742923083941</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12:27:34</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>92.9750562342219</v>
+      </c>
+      <c r="G15" t="n">
+        <v>65.77138664733151</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12:30:34</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>97.15916212822721</v>
+      </c>
+      <c r="G16" t="n">
+        <v>54.99891500210524</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug and added upload
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -1115,7 +1115,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1593,6 +1593,37 @@
         <v>54.99891500210524</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21:17:22</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>96.5882061718065</v>
+      </c>
+      <c r="G17" t="n">
+        <v>58.96413616731667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added updated encoding and encode script
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -13,6 +13,7 @@
     <sheet name="2020-11-10" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="2020-11-11" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="2020-11-12" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2020-11-14" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2144,4 +2145,184 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>16:07:22</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.75047190698253</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>16:09:49</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>94.55808920791817</v>
+      </c>
+      <c r="G3" t="n">
+        <v>57.20660651222352</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>16:10:54</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>93.31806497949607</v>
+      </c>
+      <c r="G4" t="n">
+        <v>69.20471482450479</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>16:12:47</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>94.42039855332457</v>
+      </c>
+      <c r="G5" t="n">
+        <v>51.60096886331338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue of queue
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -1552,7 +1552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,6 +1766,47 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>15:41:33</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>93.81816225047248</v>
+      </c>
+      <c r="G6" t="n">
+        <v>55.61066115619608</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>

<commit_message>
added automatic face box maker
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -17,6 +17,7 @@
     <sheet name="2020-11-16" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2020-11-20" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="2020-11-21" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2020-11-22" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1817,6 +1818,195 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>15:39:52</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>99.39610093014164</v>
+      </c>
+      <c r="G2" t="n">
+        <v>91.95237785286318</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>15:50:06</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>99.90177444071958</v>
+      </c>
+      <c r="G3" t="n">
+        <v>77.41913432818548</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15:52:45</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>99.32331759328801</v>
+      </c>
+      <c r="G4" t="n">
+        <v>62.54781983834307</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
trained, added excel for unknown,added spo2 flash
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -19,6 +19,7 @@
     <sheet name="2020-11-21" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="2020-11-22" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="2020-11-26" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="2020-11-27" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2156,6 +2157,277 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>00:15:25</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>98.2410200777593</v>
+      </c>
+      <c r="G2" t="n">
+        <v>64.12281009995567</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>00:18:19</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>97.95162681117016</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>00:20:54</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>97.87804508522433</v>
+      </c>
+      <c r="G4" t="n">
+        <v>66.84032472851912</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>00:25:04</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>96.27875888965946</v>
+      </c>
+      <c r="G5" t="n">
+        <v>63.44762551053533</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>00:29:14</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>97.6024606325315</v>
+      </c>
+      <c r="G6" t="n">
+        <v>66.86134448778704</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added dishant into training set and trained
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -2163,7 +2163,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2418,6 +2418,129 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>02:02:54</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>99.88070376432579</v>
+      </c>
+      <c r="G7" t="n">
+        <v>57.52758683819931</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>02:04:38</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>97.03971006047878</v>
+      </c>
+      <c r="G8" t="n">
+        <v>89.00981767428932</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>02:06:08</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>98.84141964022119</v>
+      </c>
+      <c r="G9" t="n">
+        <v>82.47545924642802</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>

<commit_message>
added averaging of hr
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -21,6 +21,9 @@
     <sheet name="2020-11-26" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="2020-11-27" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="2020-11-30" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="2020-12-18" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="2020-12-19" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="2020-12-21" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2659,6 +2662,2869 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>11:45:19</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.24073826351768</v>
+      </c>
+      <c r="G2" t="n">
+        <v>51.70537615717722</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>11:52:42</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>97.11718333179675</v>
+      </c>
+      <c r="G3" t="n">
+        <v>52.72670563691987</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>14:07:27</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>97.27573058703932</v>
+      </c>
+      <c r="G4" t="n">
+        <v>53.96571245471256</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15:36:02</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>96.45313273939155</v>
+      </c>
+      <c r="G5" t="n">
+        <v>74.33203207319676</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>15:38:53</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>97.34154820610669</v>
+      </c>
+      <c r="G6" t="n">
+        <v>57.96816762519403</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>15:46:33</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>96.5010981181405</v>
+      </c>
+      <c r="G7" t="n">
+        <v>53.20949625525229</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>15:57:22</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>97.37027754112241</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>15:59:12</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>97.20563133730388</v>
+      </c>
+      <c r="G9" t="n">
+        <v>70.2478186905051</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16:00:23</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>97.99015105102316</v>
+      </c>
+      <c r="G10" t="n">
+        <v>72.82620605119043</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>16:02:42</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>96.85999237239457</v>
+      </c>
+      <c r="G11" t="n">
+        <v>67.78361940097486</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16:04:10</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>97.19665329235316</v>
+      </c>
+      <c r="G12" t="n">
+        <v>67.87588256971605</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16:08:23</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>97.38239196794335</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>16:09:57</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>97.51277780048943</v>
+      </c>
+      <c r="G14" t="n">
+        <v>52.75163245856483</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>16:10:43</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>97.4881684533796</v>
+      </c>
+      <c r="G15" t="n">
+        <v>63.06409973316579</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>16:11:53</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>97.39352882693342</v>
+      </c>
+      <c r="G16" t="n">
+        <v>67.41213656406872</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16:13:10</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>97.71600752506725</v>
+      </c>
+      <c r="G17" t="n">
+        <v>70.02086401232403</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>16:16:00</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>96.54155981981003</v>
+      </c>
+      <c r="G18" t="n">
+        <v>57.76684290080195</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>16:17:14</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>97.72419482932426</v>
+      </c>
+      <c r="G19" t="n">
+        <v>67.24411547232681</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>16:17:46</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>97.06172870512405</v>
+      </c>
+      <c r="G20" t="n">
+        <v>69.82111121018396</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>16:19:18</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>98.01307949806751</v>
+      </c>
+      <c r="G21" t="n">
+        <v>55.81616272367665</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>16:22:36</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>97.82100257037293</v>
+      </c>
+      <c r="G22" t="n">
+        <v>78.23681775057739</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>16:23:30</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>96.89322929408749</v>
+      </c>
+      <c r="G23" t="n">
+        <v>57.35779012831677</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>16:24:02</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>97.69409803578974</v>
+      </c>
+      <c r="G24" t="n">
+        <v>56.22943589274003</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>16:25:58</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>97.45975929870087</v>
+      </c>
+      <c r="G25" t="n">
+        <v>50.81727161427492</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>16:27:30</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>97.60689138953293</v>
+      </c>
+      <c r="G26" t="n">
+        <v>57.90969305269116</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>16:28:17</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>96.5911635824157</v>
+      </c>
+      <c r="G27" t="n">
+        <v>62.41421568282817</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>16:49:38</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>96.62755411029967</v>
+      </c>
+      <c r="G28" t="n">
+        <v>63.78822150967764</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>17:02:16</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>97.76202421406589</v>
+      </c>
+      <c r="G29" t="n">
+        <v>63.44509846499194</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>17:04:15</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>98.18314921709099</v>
+      </c>
+      <c r="G30" t="n">
+        <v>79.18106258725447</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>20:09:38</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>97.26926247047665</v>
+      </c>
+      <c r="G31" t="n">
+        <v>87.15025319334836</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>20:10:48</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>92.57335200462954</v>
+      </c>
+      <c r="G32" t="n">
+        <v>125.0457659672676</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>20:11:44</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>61.461566639</v>
+      </c>
+      <c r="G33" t="n">
+        <v>89.97708520222305</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>20:14:32</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>95.65414764539668</v>
+      </c>
+      <c r="G34" t="n">
+        <v>131.7865754611464</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>20:15:09</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>96.43804004303492</v>
+      </c>
+      <c r="G35" t="n">
+        <v>85.21769304194731</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12:03:12</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>96.87411645891605</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100.4374790370737</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>12:04:38</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>96.76756349909522</v>
+      </c>
+      <c r="G3" t="n">
+        <v>78.09162899725925</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12:29:36</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>96.72793434791868</v>
+      </c>
+      <c r="G4" t="n">
+        <v>81.95522081579777</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12:31:25</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>97.15616893200558</v>
+      </c>
+      <c r="G5" t="n">
+        <v>63.75159453951373</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>12:34:09</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>97.55439473661806</v>
+      </c>
+      <c r="G6" t="n">
+        <v>63.20751243189989</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>12:34:41</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>99.16490687297323</v>
+      </c>
+      <c r="G7" t="n">
+        <v>89.69692291906223</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12:35:10</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>95.30940015995125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>64.00483237920305</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12:35:39</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>96.82845075372529</v>
+      </c>
+      <c r="G9" t="n">
+        <v>166.2661704755468</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>12:37:32</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>97.00161821718108</v>
+      </c>
+      <c r="G10" t="n">
+        <v>64.77139779587156</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12:38:21</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>98.59397335134653</v>
+      </c>
+      <c r="G11" t="n">
+        <v>96.56732224311034</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12:46:48</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>97.16053048553847</v>
+      </c>
+      <c r="G12" t="n">
+        <v>83.17156942398016</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12:50:13</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>97.53366749712616</v>
+      </c>
+      <c r="G13" t="n">
+        <v>52.34858322789545</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12:53:52</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>97.45659852771519</v>
+      </c>
+      <c r="G14" t="n">
+        <v>56.75328427114411</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12:58:38</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>97.63551808241124</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>13:01:31</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>97.54246979678044</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>13:03:37</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>96.60784699695392</v>
+      </c>
+      <c r="G17" t="n">
+        <v>52.12003531031747</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>13:05:56</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>96.331594382362</v>
+      </c>
+      <c r="G18" t="n">
+        <v>54.01383627812329</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>13:08:56</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>97.35715058156813</v>
+      </c>
+      <c r="G19" t="n">
+        <v>61.43193775161463</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>13:19:35</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>96.54978510089842</v>
+      </c>
+      <c r="G20" t="n">
+        <v>59.61935723090035</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>13:22:40</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>97.30782035925692</v>
+      </c>
+      <c r="G21" t="n">
+        <v>57.97437324803824</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>13:27:30</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>97.68299651287535</v>
+      </c>
+      <c r="G22" t="n">
+        <v>54.89471174220493</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>13:46:55</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>98.36833460929572</v>
+      </c>
+      <c r="G23" t="n">
+        <v>102.6429967535731</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>13:53:24</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>97.13918310801917</v>
+      </c>
+      <c r="G24" t="n">
+        <v>99.74136652485188</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>14:13:19</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>96.87856647482712</v>
+      </c>
+      <c r="G25" t="n">
+        <v>79.71977859433257</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>14:18:54</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>98.05964102067543</v>
+      </c>
+      <c r="G26" t="n">
+        <v>149.6676586322658</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>14:44:49</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>97.44163715262545</v>
+      </c>
+      <c r="G27" t="n">
+        <v>127.6146340211577</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>14:51:24</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>99.0203762365728</v>
+      </c>
+      <c r="G28" t="n">
+        <v>75.32927520928729</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>14:51:51</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>96.85472952500093</v>
+      </c>
+      <c r="G29" t="n">
+        <v>77.2084422047251</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>14:56:06</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>94.36255176781209</v>
+      </c>
+      <c r="G30" t="n">
+        <v>66.53555332158072</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>14:58:29</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>98.04462782788009</v>
+      </c>
+      <c r="G31" t="n">
+        <v>143.2182048603935</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>15:56:01</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.427853687173</v>
+      </c>
+      <c r="G2" t="n">
+        <v>59.68131193891786</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added ratio feature for various display sizes
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -24,6 +24,7 @@
     <sheet name="2020-12-18" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="2020-12-19" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2020-12-21" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="2020-12-27" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -5525,6 +5526,113 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10:45:04</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>95.83510336095262</v>
+      </c>
+      <c r="G2" t="n">
+        <v>67.90663936802549</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Fixed auto button problem
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -25,6 +25,7 @@
     <sheet name="2020-12-19" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2020-12-21" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="2020-12-27" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="2021-01-01" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -5740,6 +5741,277 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>18:35:31</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>98.20766575855964</v>
+      </c>
+      <c r="G2" t="n">
+        <v>147.3157019226992</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>18:40:25</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>96.85625977255769</v>
+      </c>
+      <c r="G3" t="n">
+        <v>92.28159635919941</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>18:43:09</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>95.5139015649184</v>
+      </c>
+      <c r="G4" t="n">
+        <v>130.9243342687308</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>18:53:17</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>97.63219807251328</v>
+      </c>
+      <c r="G5" t="n">
+        <v>156.8040310916165</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>18:54:01</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>97.80702465077516</v>
+      </c>
+      <c r="G6" t="n">
+        <v>109.9791580367084</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
shifted email from local code to node js code
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -27,6 +27,8 @@
     <sheet name="2020-12-27" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="2021-01-01" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="2021-01-04" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="2021-01-05" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="2021-01-06" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -6161,6 +6163,630 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>23:15:01</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.94802944634111</v>
+      </c>
+      <c r="G2" t="n">
+        <v>97.15533902413459</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>23:17:25</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>96.72572416450372</v>
+      </c>
+      <c r="G3" t="n">
+        <v>67.29117181934262</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>23:20:08</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>97.01874773506313</v>
+      </c>
+      <c r="G4" t="n">
+        <v>72.38625543168776</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>23:22:31</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>97.5138432365595</v>
+      </c>
+      <c r="G5" t="n">
+        <v>62.76942121792798</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>23:40:33</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>97.62289986582616</v>
+      </c>
+      <c r="G6" t="n">
+        <v>77.90709489973645</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>23:45:52</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>98.17296855471439</v>
+      </c>
+      <c r="G7" t="n">
+        <v>89.27848258751145</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>23:46:49</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>97.34296827829047</v>
+      </c>
+      <c r="G8" t="n">
+        <v>122.767066460571</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>23:51:16</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>97.77812564676016</v>
+      </c>
+      <c r="G9" t="n">
+        <v>114.6530935674223</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>00:02:34</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.67929655448826</v>
+      </c>
+      <c r="G2" t="n">
+        <v>99.77017618367501</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>00:05:03</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>97.24904921482502</v>
+      </c>
+      <c r="G3" t="n">
+        <v>70.90286282809069</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>00:07:03</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>97.96449387111554</v>
+      </c>
+      <c r="G4" t="n">
+        <v>108.0425018446584</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>00:17:04</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>97.03484786647245</v>
+      </c>
+      <c r="G5" t="n">
+        <v>69.14380743344644</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
fixed face box not changing
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -6563,7 +6563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6777,6 +6777,129 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>14:18:15</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>96.6712521745384</v>
+      </c>
+      <c r="G6" t="n">
+        <v>56.68526035361902</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14:20:23</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>97.15096348632157</v>
+      </c>
+      <c r="G7" t="n">
+        <v>77.93673309236452</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14:20:42</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>94.97829344384658</v>
+      </c>
+      <c r="G8" t="n">
+        <v>80.72980249297832</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>

<commit_message>
improved fr and excel engine
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2021-01-07" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-01-07" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-01-11" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +55,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -434,7 +435,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -541,6 +542,441 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Compensated</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>18:35:14</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.59385534014351</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>19:31:51</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>97.66750902355957</v>
+      </c>
+      <c r="G3" t="n">
+        <v>66.57590464616032</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>19:36:47</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>97.26071028597477</v>
+      </c>
+      <c r="G4" t="n">
+        <v>85.7017862963194</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>19:40:10</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>97.38368981463954</v>
+      </c>
+      <c r="G5" t="n">
+        <v>70.06637470606302</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>19:44:27</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>96.9643448485741</v>
+      </c>
+      <c r="G6" t="n">
+        <v>131.0042587766994</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>19:44:46</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>97.66721486857014</v>
+      </c>
+      <c r="G7" t="n">
+        <v>124.4869430863692</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>19:46:16</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>97.2858232863867</v>
+      </c>
+      <c r="G8" t="n">
+        <v>51.98913957578586</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>19:47:30</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>97.47390529427025</v>
+      </c>
+      <c r="G9" t="n">
+        <v>94.44407387681979</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>301/Sanskruti-1,Andheri, Mumbai</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>19:47:59</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>97.60036380894805</v>
+      </c>
+      <c r="G10" t="n">
+        <v>74.83467442504315</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all unkown support in excel
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -9,6 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-01-07" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-01-11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-01-28" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1020,4 +1021,111 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Face_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Body_temp</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>18:22:27</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>97.47302216588803</v>
+      </c>
+      <c r="G2" t="n">
+        <v>88.02019999234678</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>